<commit_message>
fixed a bug on debut and end date in add month page
</commit_message>
<xml_diff>
--- a/bug report.xlsx
+++ b/bug report.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/bc10114a77d9812e/Projets_Personnels/budget-management-app/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\antoi\OneDrive\Projets_Personnels\budget-management-app\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="19" documentId="11_AD4D9D64A577C15A4A54182A181B75F85ADEDD85" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2578E0E0-DB12-4E89-BA86-7278322CDC24}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAA75193-CE2F-4200-BE99-119B1EA91891}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="12">
   <si>
     <t>Date</t>
   </si>
@@ -55,6 +55,12 @@
   </si>
   <si>
     <t>NON</t>
+  </si>
+  <si>
+    <t>Single-month/details</t>
+  </si>
+  <si>
+    <t>Les catégories et le camembert ne s'affiche pas</t>
   </si>
 </sst>
 </file>
@@ -379,20 +385,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:F3"/>
+  <dimension ref="A2:F4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="45.42578125" customWidth="1"/>
+    <col min="1" max="1" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="45.44140625" customWidth="1"/>
+    <col min="5" max="6" width="9.109375" style="3"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -405,14 +412,14 @@
       <c r="D2" t="s">
         <v>3</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" s="3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>44408</v>
       </c>
@@ -429,6 +436,26 @@
         <v>8</v>
       </c>
       <c r="F3" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" s="1">
+        <v>44493</v>
+      </c>
+      <c r="B4">
+        <v>2</v>
+      </c>
+      <c r="C4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="F4" s="3" t="s">
         <v>9</v>
       </c>
     </row>

</xml_diff>